<commit_message>
Añadido método de la secante
</commit_message>
<xml_diff>
--- a/Metodos B Ps NR S.xlsx
+++ b/Metodos B Ps NR S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeron\Documents\MAC\Métodos Númericos I\Métodos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140B60AA-39F6-4F24-B34B-B3E8C816B7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF854991-B720-49A8-9291-DE47944D1E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>tabla por metodo de biseccion</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Para C</t>
+  </si>
+  <si>
+    <t>f(x)=x^4-3x^3+3x-0.5</t>
   </si>
 </sst>
 </file>
@@ -137,8 +140,8 @@
     <numFmt numFmtId="168" formatCode="0.000000000000000"/>
     <numFmt numFmtId="169" formatCode="0.0000000"/>
     <numFmt numFmtId="170" formatCode="0.0000000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="171" formatCode="0.00000000"/>
+    <numFmt numFmtId="172" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -178,8 +181,8 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1559,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6064B852-2034-4FF9-A1AE-99CE07290829}">
-  <dimension ref="B3:H29"/>
+  <dimension ref="B3:H33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,27 +2060,166 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D28" s="1">
+        <f>POWER(C28,4)-3*POWER(C28,3)+3*C28-0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="E28">
+        <f>4*POWER(C28,3)-9*POWER(C28,2)+3</f>
+        <v>-10</v>
+      </c>
+      <c r="F28" s="4">
+        <f>C28-D28/E28</f>
+        <v>-0.95</v>
+      </c>
+      <c r="G28" s="5">
+        <f>ABS((F28-C28)/(F28))</f>
+        <v>5.2631578947368474E-2</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" ref="H28:H33" si="16">G28*100</f>
+        <v>5.2631578947368478</v>
+      </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="B29">
+        <f>B28+1</f>
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" ref="C29:C33" si="17">F28</f>
+        <v>-0.95</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" ref="D29:D33" si="18">POWER(C29,4)-3*POWER(C29,3)+3*C29-0.5</f>
+        <v>3.6631250000000115E-2</v>
+      </c>
+      <c r="E29">
+        <f>4*POWER(C29,3)-9*POWER(C29,2)+3</f>
+        <v>-8.5519999999999996</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" ref="F28:F33" si="19">C29-D29/E29</f>
+        <v>-0.94571664522918608</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" ref="G29:G31" si="20">ABS((F29-C29)/(F29))</f>
+        <v>4.5292157988567928E-3</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="16"/>
+        <v>0.45292157988567927</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f t="shared" ref="B30:B33" si="21">B29+1</f>
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="17"/>
+        <v>-0.94571664522918608</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="18"/>
+        <v>2.5568358707150907E-4</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E29:E33" si="22">4*POWER(C30,3)-9*POWER(C30,2)+3</f>
+        <v>-8.4327398683152239</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="19"/>
+        <v>-0.94568632488359683</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="20"/>
+        <v>3.2061736319370056E-5</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="16"/>
+        <v>3.2061736319370054E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <f>F30</f>
+        <v>-0.94568632488359683</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="18"/>
+        <v>1.2757932044138443E-8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="22"/>
+        <v>-8.4318983319043674</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="19"/>
+        <v>-0.94568632337054115</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="20"/>
+        <v>1.5999551260862259E-9</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="16"/>
+        <v>1.5999551260862258E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2089,18 +2231,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36AA98C-632E-45E0-8459-D3C1E04AE844}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="3.77734375" customWidth="1"/>
     <col min="3" max="6" width="18.77734375" customWidth="1"/>
     <col min="7" max="7" width="20.77734375" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
@@ -2201,7 +2344,7 @@
         <v>-0.34017593563442827</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" ref="G5:G8" si="2">D5-(F5)*(D5-C5)/(F5-E5)</f>
+        <f t="shared" ref="G5:G7" si="2">D5-(F5)*(D5-C5)/(F5-E5)</f>
         <v>0.76174018458685488</v>
       </c>
       <c r="H5" s="2">
@@ -2216,14 +2359,14 @@
         <f t="shared" ref="J5:J8" si="5">I5/G5</f>
         <v>3.6413126963092859E-2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="7">
         <f t="shared" ref="K5:K8" si="6">J5*100</f>
         <v>3.6413126963092859</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6">
-        <f t="shared" ref="B6:B20" si="7">B5+1</f>
+        <f t="shared" ref="B6:B8" si="7">B5+1</f>
         <v>3</v>
       </c>
       <c r="C6" s="5">
@@ -2258,7 +2401,7 @@
         <f t="shared" si="5"/>
         <v>4.1876422272068203E-3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="7">
         <f t="shared" si="6"/>
         <v>0.41876422272068203</v>
       </c>
@@ -2300,7 +2443,7 @@
         <f t="shared" si="5"/>
         <v>5.2973911677294769E-5</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="7">
         <f t="shared" si="6"/>
         <v>5.2973911677294773E-3</v>
       </c>
@@ -2327,7 +2470,7 @@
         <v>-8.159522577599887E-7</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" si="2"/>
+        <f>D8-(F8)*(D8-C8)/(F8-E8)</f>
         <v>0.75860370478839767</v>
       </c>
       <c r="H8" s="2">
@@ -2342,7 +2485,7 @@
         <f t="shared" si="5"/>
         <v>9.6334269376068881E-8</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="7">
         <f t="shared" si="6"/>
         <v>9.6334269376068878E-6</v>
       </c>

</xml_diff>